<commit_message>
create user delete & edit functions
</commit_message>
<xml_diff>
--- a/excel/sample_excel.xlsx
+++ b/excel/sample_excel.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="388">
   <si>
     <t>name</t>
   </si>
@@ -674,15 +674,6 @@
     <t>XPFU</t>
   </si>
   <si>
-    <t>Adenike</t>
-  </si>
-  <si>
-    <t>Adesokan</t>
-  </si>
-  <si>
-    <t>pSjS</t>
-  </si>
-  <si>
     <t>Maike</t>
   </si>
   <si>
@@ -1167,6 +1158,21 @@
   </si>
   <si>
     <t>IrIB</t>
+  </si>
+  <si>
+    <t>harshi</t>
+  </si>
+  <si>
+    <t>u0002</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t>jjj</t>
+  </si>
+  <si>
+    <t>kkk</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1220,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GZ61"/>
+  <dimension ref="A1:GZ62"/>
   <cols>
     <col min="1" max="1" width="10"/>
     <col min="2" max="2" width="17"/>
@@ -2533,10 +2539,10 @@
         <v>293</v>
       </c>
       <c r="B30" t="s">
+        <v>291</v>
+      </c>
+      <c r="C30" t="s">
         <v>294</v>
-      </c>
-      <c r="C30" t="s">
-        <v>295</v>
       </c>
       <c r="D30" t="s" s="2">
         <v>211</v>
@@ -2547,10 +2553,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>295</v>
+      </c>
+      <c r="B31" t="s">
         <v>296</v>
-      </c>
-      <c r="B31" t="s">
-        <v>294</v>
       </c>
       <c r="C31" t="s">
         <v>297</v>
@@ -2703,10 +2709,10 @@
         <v>322</v>
       </c>
       <c r="B40" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" t="s">
         <v>323</v>
-      </c>
-      <c r="C40" t="s">
-        <v>324</v>
       </c>
       <c r="D40" t="s" s="2">
         <v>211</v>
@@ -2717,10 +2723,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>324</v>
+      </c>
+      <c r="B41" t="s">
         <v>325</v>
-      </c>
-      <c r="B41" t="s">
-        <v>294</v>
       </c>
       <c r="C41" t="s">
         <v>326</v>
@@ -2768,13 +2774,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>313</v>
+      </c>
+      <c r="B44" t="s">
         <v>333</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>334</v>
-      </c>
-      <c r="C44" t="s">
-        <v>335</v>
       </c>
       <c r="D44" t="s" s="2">
         <v>211</v>
@@ -2785,7 +2791,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="B45" t="s">
         <v>336</v>
@@ -3060,15 +3066,32 @@
         <v>383</v>
       </c>
       <c r="B61" t="s">
+        <v>383</v>
+      </c>
+      <c r="C61" t="s">
         <v>384</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="E61">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
         <v>385</v>
       </c>
-      <c r="D61" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="E61">
+      <c r="B62" t="s">
+        <v>386</v>
+      </c>
+      <c r="C62" t="s">
+        <v>387</v>
+      </c>
+      <c r="D62" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="E62">
         <v>2022</v>
       </c>
     </row>

</xml_diff>